<commit_message>
Addiding the Project with Whole Test cases
</commit_message>
<xml_diff>
--- a/FileInput/DataEngine.xlsx
+++ b/FileInput/DataEngine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saqui\eclipse\eslipse-work space\Hybrid_FrameWork\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01002450-E3AD-480F-9F94-18444CE3E86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FA29E1-DF1D-4CB2-AE2B-393E5CF8A99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="167">
   <si>
     <t>TCID</t>
   </si>
@@ -531,9 +531,6 @@
   </si>
   <si>
     <t>//input[@placeholder='Customer Name']</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -675,12 +672,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -980,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -1026,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -1038,7 +1034,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -1074,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D95523-9861-4BEC-B077-671207A6FABA}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,7 +1245,7 @@
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="1"/>
@@ -1289,27 +1285,6 @@
         <v>22</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1336,180 +1311,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>10</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="7"/>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>10</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E10" s="1">
@@ -1518,34 +1493,34 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E12" s="1">
@@ -1554,34 +1529,34 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="1">
@@ -1590,52 +1565,52 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="1">
@@ -1644,34 +1619,34 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>77</v>
       </c>
       <c r="E19" s="1">
@@ -1680,76 +1655,76 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="C21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>70</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="7"/>
+      <c r="E22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="7"/>
+      <c r="C23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1776,546 +1751,546 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>10</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>10</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>10</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="10"/>
+      <c r="E11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>10</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="10"/>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>10</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>1</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="10"/>
+      <c r="E17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>2</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="10"/>
+      <c r="E23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="C24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>10</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="C25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="10"/>
+      <c r="E25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="C26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>10</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="10"/>
+      <c r="E27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="10"/>
+      <c r="C28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="8"/>
+      <c r="E29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="8"/>
+      <c r="C30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2362,562 +2337,562 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="12"/>
+      <c r="C2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="12"/>
+      <c r="C3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>10</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="12"/>
+      <c r="E7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>10</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>10</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="12"/>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>10</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="12"/>
+      <c r="E13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>10</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="12"/>
+      <c r="E15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <v>9876543212</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="11">
         <v>9876541232</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="F24" s="12"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="12"/>
+      <c r="E25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="11">
         <v>10</v>
       </c>
-      <c r="F26" s="12"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="12"/>
+      <c r="E27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="C28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="11">
         <v>10</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="C29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="12"/>
+      <c r="E29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="12"/>
+      <c r="C30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="C31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="12"/>
+      <c r="E31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="12"/>
+      <c r="C32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2966,562 +2941,562 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="12"/>
+      <c r="C2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="12"/>
+      <c r="C3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>10</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="12"/>
+      <c r="E7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>10</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>10</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="12"/>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>10</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="12"/>
+      <c r="E13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>10</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="12"/>
+      <c r="E15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <v>1234567898</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="11">
         <v>9876543215</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="F24" s="12"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="12"/>
+      <c r="E25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="11">
         <v>10</v>
       </c>
-      <c r="F26" s="12"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="12"/>
+      <c r="E27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="C28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="11">
         <v>10</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="C29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="12"/>
+      <c r="E29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="12"/>
+      <c r="C30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="C31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="12"/>
+      <c r="E31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="12"/>
+      <c r="C32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>